<commit_message>
Updated V1.3 files, I2C address error and Pinout files
Updated gitignore file
Updated pinout with the error on the Power Enable of each camera
Corrected the Barometric pressure I2C address
</commit_message>
<xml_diff>
--- a/IRIS2/01-Design/IRIS2_PCB_CPU/docs/IRIS2_pinouts.xlsx
+++ b/IRIS2/01-Design/IRIS2_PCB_CPU/docs/IRIS2_pinouts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\schematics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\IRIS2_PCB_CPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C82BD77-D0AF-4647-BDD1-8C4D331C5512}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2AD52A-FEFC-4A42-92A2-CFF57F4006B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -908,12 +908,6 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -927,6 +921,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Bad" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1447,8 +1447,8 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1461,1306 +1461,1306 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <f t="shared" ref="A3:A34" si="0">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+      <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+      <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+      <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
+      <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
+      <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
+      <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
+      <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
+      <c r="A35" s="2">
         <f t="shared" ref="A35:A66" si="1">A34+1</f>
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
+      <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
+      <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
+      <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
+      <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
+      <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="4">
+      <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
+      <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="4">
+      <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="4">
+      <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="4">
+      <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="4">
+      <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
+      <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
+      <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
+      <c r="A49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
+      <c r="A50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+      <c r="A51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
+      <c r="A52" s="2">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+      <c r="A53" s="2">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
+      <c r="A54" s="2">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="4">
+      <c r="A55" s="2">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="4">
+      <c r="A56" s="2">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="4">
+      <c r="A57" s="2">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
+      <c r="A58" s="2">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E60" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="4">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="4">
-        <f t="shared" si="1"/>
-        <v>59</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="4">
+      <c r="A61" s="2">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="4">
+      <c r="A62" s="2">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D62" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="4">
+      <c r="A63" s="2">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="2" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="4">
+      <c r="A64" s="2">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="2" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="4">
+      <c r="A65" s="2">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="2" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="4">
+      <c r="A66" s="2">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="4">
+      <c r="A67" s="2">
         <f t="shared" ref="A67:A81" si="2">A66+1</f>
         <v>66</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="2" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="4">
+      <c r="A68" s="2">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" s="2" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="4">
+      <c r="A69" s="2">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D69" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="2" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="4">
+      <c r="A70" s="2">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="4">
+      <c r="A71" s="2">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="4">
+      <c r="A72" s="2">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="4">
+      <c r="A73" s="2">
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="4">
+      <c r="A74" s="2">
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="4">
+      <c r="A75" s="2">
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="4">
+      <c r="A76" s="2">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="4">
+      <c r="A77" s="2">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C77" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D77" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E77" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="4">
+      <c r="A78" s="2">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="4">
+      <c r="A79" s="2">
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E79" s="4" t="s">
+      <c r="E79" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="4">
+      <c r="A80" s="2">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E80" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="4">
+      <c r="A81" s="2">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D81" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2795,800 +2795,800 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="I1" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="11" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="2">
         <v>1</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="2">
         <v>2</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="2">
         <v>2</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="2">
         <v>3</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>4</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>4</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="2">
         <v>4</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="I7" s="4">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="I7" s="2">
         <v>5</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="2">
         <v>5</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="I8" s="4">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="I8" s="2">
         <v>6</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="2">
         <v>6</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="2">
         <v>7</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="2">
         <v>7</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="2">
         <v>8</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="2">
         <v>8</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
         <v>2</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="2">
         <v>9</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>3</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="2">
         <v>10</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
+      <c r="K12" s="2"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="E13" s="4">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="E13" s="2">
         <v>4</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="E15" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="I15" s="1" t="s">
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="I15" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="11" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <v>1</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="I17" s="4">
+      <c r="G17" s="2"/>
+      <c r="I17" s="2">
         <v>1</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <v>2</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="I18" s="4">
+      <c r="G18" s="2"/>
+      <c r="I18" s="2">
         <v>2</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>3</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <v>3</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="I19" s="4">
+      <c r="G19" s="2"/>
+      <c r="I19" s="2">
         <v>3</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <v>4</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <v>4</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="I20" s="4">
+      <c r="G20" s="2"/>
+      <c r="I20" s="2">
         <v>4</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
+      <c r="A21" s="2">
         <v>5</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <v>5</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="I21" s="4">
+      <c r="G21" s="2"/>
+      <c r="I21" s="2">
         <v>5</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="A22" s="2">
         <v>6</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="2">
         <v>6</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="4">
+      <c r="G22" s="2"/>
+      <c r="I22" s="2">
         <v>6</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="A23" s="2">
         <v>7</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="2">
         <v>7</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="I23" s="4">
+      <c r="G23" s="2"/>
+      <c r="I23" s="2">
         <v>7</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="A24" s="2">
         <v>8</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="2">
         <v>8</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="I24" s="4">
+      <c r="G24" s="2"/>
+      <c r="I24" s="2">
         <v>8</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
+      <c r="A25" s="2">
         <v>9</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="2">
         <v>9</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="I25" s="4">
+      <c r="G25" s="2"/>
+      <c r="I25" s="2">
         <v>9</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26" s="2">
         <v>10</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
+      <c r="A27" s="2">
         <v>11</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28" s="2">
         <v>12</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+      <c r="A29" s="2">
         <v>13</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+      <c r="A30" s="2">
         <v>14</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
+      <c r="A31" s="2">
         <v>15</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>182</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="E8:G8"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="E8:G8"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3618,160 +3618,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="I1" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="11" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="2">
         <v>2</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>4</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>4</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="2" t="s">
         <v>187</v>
       </c>
       <c r="L6" t="s">
@@ -3779,31 +3779,31 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>5</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="2">
         <v>5</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L7" t="s">
@@ -3811,526 +3811,526 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>6</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="2">
         <v>6</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>7</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>8</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="E15" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="I15" s="1" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="I15" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="11" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <f t="shared" ref="E17:G24" si="0">E3</f>
         <v>1</v>
       </c>
-      <c r="F17" s="4" t="str">
+      <c r="F17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GND</v>
       </c>
-      <c r="G17" s="4" t="str">
+      <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="2">
         <v>1</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="K17" s="4"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F18" s="4" t="str">
+      <c r="F18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GND</v>
       </c>
-      <c r="G18" s="4" t="str">
+      <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="2">
         <v>2</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="K18" s="4"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>3</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F19" s="4" t="str">
+      <c r="F19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>5V</v>
       </c>
-      <c r="G19" s="4" t="str">
+      <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="2">
         <v>3</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <v>4</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F20" s="4" t="str">
+      <c r="F20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>5V</v>
       </c>
-      <c r="G20" s="4" t="str">
+      <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="2">
         <v>4</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="K20" s="4"/>
+      <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F21" s="4" t="str">
+      <c r="F21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UART Tx</v>
       </c>
-      <c r="G21" s="4" t="str">
+      <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="2">
         <v>5</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K21" s="4"/>
+      <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E22" s="4">
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F22" s="4" t="str">
+      <c r="F22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UART Rx</v>
       </c>
-      <c r="G22" s="4" t="str">
+      <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>In</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="2">
         <v>6</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K22" s="4"/>
+      <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E23" s="4">
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F23" s="4" t="str">
+      <c r="F23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Power On</v>
       </c>
-      <c r="G23" s="4" t="str">
+      <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="2">
         <v>7</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K23" s="4"/>
+      <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E24" s="4">
+      <c r="E24" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F24" s="4" t="str">
+      <c r="F24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Power Status</v>
       </c>
-      <c r="G24" s="4" t="str">
+      <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>In</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="2">
         <v>8</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="K24" s="4"/>
+      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="I25" s="4">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="I25" s="2">
         <v>9</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="4"/>
+      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="I26" s="4">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="I26" s="2">
         <v>10</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K26" s="4"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I27" s="4">
+      <c r="I27" s="2">
         <v>11</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="K27" s="4"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I28" s="4">
+      <c r="I28" s="2">
         <v>12</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K28" s="4"/>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="I29" s="4">
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="I29" s="2">
         <v>13</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K29" s="4"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="2">
         <v>14</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K30" s="4"/>
+      <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E31" s="4">
+      <c r="E31" s="2">
         <f t="shared" ref="E31:G38" si="1">E3</f>
         <v>1</v>
       </c>
-      <c r="F31" s="4" t="str">
+      <c r="F31" s="2" t="str">
         <f t="shared" si="1"/>
         <v>GND</v>
       </c>
-      <c r="G31" s="4" t="str">
+      <c r="G31" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E32" s="4">
+      <c r="E32" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F32" s="4" t="str">
+      <c r="F32" s="2" t="str">
         <f t="shared" si="1"/>
         <v>GND</v>
       </c>
-      <c r="G32" s="4" t="str">
+      <c r="G32" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E33" s="4">
+      <c r="E33" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F33" s="4" t="str">
+      <c r="F33" s="2" t="str">
         <f t="shared" si="1"/>
         <v>5V</v>
       </c>
-      <c r="G33" s="4" t="str">
+      <c r="G33" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E34" s="4">
+      <c r="E34" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F34" s="4" t="str">
+      <c r="F34" s="2" t="str">
         <f t="shared" si="1"/>
         <v>5V</v>
       </c>
-      <c r="G34" s="4" t="str">
+      <c r="G34" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E35" s="4">
+      <c r="E35" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F35" s="4" t="str">
+      <c r="F35" s="2" t="str">
         <f t="shared" si="1"/>
         <v>UART Tx</v>
       </c>
-      <c r="G35" s="4" t="str">
+      <c r="G35" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E36" s="4">
+      <c r="E36" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F36" s="4" t="str">
+      <c r="F36" s="2" t="str">
         <f t="shared" si="1"/>
         <v>UART Rx</v>
       </c>
-      <c r="G36" s="4" t="str">
+      <c r="G36" s="2" t="str">
         <f t="shared" si="1"/>
         <v>In</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E37" s="4">
+      <c r="E37" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="F37" s="4" t="str">
+      <c r="F37" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Power On</v>
       </c>
-      <c r="G37" s="4" t="str">
+      <c r="G37" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Out</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E38" s="4">
+      <c r="E38" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F38" s="4" t="str">
+      <c r="F38" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Power Status</v>
       </c>
-      <c r="G38" s="4" t="str">
+      <c r="G38" s="2" t="str">
         <f t="shared" si="1"/>
         <v>In</v>
       </c>

</xml_diff>

<commit_message>
Updated connector of Sunrise
</commit_message>
<xml_diff>
--- a/IRIS2/01-Design/IRIS2_PCB_CPU/docs/IRIS2_pinouts.xlsx
+++ b/IRIS2/01-Design/IRIS2_PCB_CPU/docs/IRIS2_pinouts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\IRIS2_PCB_CPU\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2AD52A-FEFC-4A42-92A2-CFF57F4006B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846F7477-4B12-4BF0-B0CC-07C90D01F50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MCU" sheetId="1" r:id="rId1"/>
@@ -674,12 +674,6 @@
     <t>DB15 Female Debug + Video</t>
   </si>
   <si>
-    <t>DB9 Female Sunrise</t>
-  </si>
-  <si>
-    <t>DB9 Male Charger</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -698,9 +692,6 @@
     <t>UART Debug</t>
   </si>
   <si>
-    <t>5V</t>
-  </si>
-  <si>
     <t>TXD</t>
   </si>
   <si>
@@ -786,6 +777,15 @@
   </si>
   <si>
     <t>Power from Camera 04 Status (Input)</t>
+  </si>
+  <si>
+    <t>3.9V</t>
+  </si>
+  <si>
+    <t>DB9 Male Sunrise</t>
+  </si>
+  <si>
+    <t>DB9 Female Charger</t>
   </si>
 </sst>
 </file>
@@ -922,10 +922,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1446,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
@@ -2470,10 +2470,10 @@
         <v>151</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2485,13 +2485,13 @@
         <v>152</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -2503,13 +2503,13 @@
         <v>153</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2557,13 +2557,13 @@
         <v>160</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2575,13 +2575,13 @@
         <v>161</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -2778,7 +2778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -2795,26 +2795,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="E1" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="I1" s="14" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="I1" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="M1" s="14" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="M1" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -3048,11 +3048,11 @@
       <c r="C8" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="I8" s="2">
         <v>6</v>
       </c>
@@ -3225,21 +3225,21 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="E15" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="I15" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="I15" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
@@ -3278,13 +3278,13 @@
         <v>184</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G17" s="2"/>
       <c r="I17" s="2">
@@ -3305,13 +3305,13 @@
         <v>189</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E18" s="2">
         <v>2</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G18" s="2"/>
       <c r="I18" s="2">
@@ -3332,7 +3332,7 @@
         <v>193</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E19" s="2">
         <v>3</v>
@@ -3359,7 +3359,7 @@
         <v>195</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E20" s="2">
         <v>4</v>
@@ -3386,7 +3386,7 @@
         <v>197</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E21" s="2">
         <v>5</v>
@@ -3413,7 +3413,7 @@
         <v>200</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E22" s="2">
         <v>6</v>
@@ -3440,7 +3440,7 @@
         <v>203</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E23" s="2">
         <v>7</v>
@@ -3467,13 +3467,13 @@
         <v>206</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E24" s="2">
         <v>8</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G24" s="2"/>
       <c r="I24" s="2">
@@ -3500,7 +3500,7 @@
         <v>9</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G25" s="2"/>
       <c r="I25" s="2">
@@ -3540,7 +3540,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>182</v>
@@ -3604,8 +3604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3618,21 +3618,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="E1" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="I1" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="E1" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="I1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
@@ -3733,7 +3733,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>183</v>
@@ -3760,7 +3760,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>183</v>
@@ -3769,13 +3769,13 @@
         <v>4</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>187</v>
       </c>
       <c r="L6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -3801,13 +3801,13 @@
         <v>5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>183</v>
       </c>
       <c r="L7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -3851,7 +3851,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>183</v>
@@ -3871,7 +3871,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>187</v>
@@ -3900,21 +3900,21 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="E15" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="I15" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="A15" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="E15" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="I15" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
@@ -3971,7 +3971,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -4001,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="K18" s="2"/>
     </row>
@@ -4021,7 +4021,7 @@
       </c>
       <c r="F19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>5V</v>
+        <v>3.9V</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4031,7 +4031,7 @@
         <v>3</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="K19" s="2"/>
     </row>
@@ -4051,7 +4051,7 @@
       </c>
       <c r="F20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>5V</v>
+        <v>3.9V</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4061,7 +4061,7 @@
         <v>4</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="K20" s="2"/>
     </row>
@@ -4145,7 +4145,7 @@
         <v>8</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K24" s="2"/>
     </row>
@@ -4192,11 +4192,11 @@
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E29" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="E29" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="I29" s="2">
         <v>13</v>
       </c>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="F33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>5V</v>
+        <v>3.9V</v>
       </c>
       <c r="G33" s="2" t="str">
         <f t="shared" si="1"/>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="F34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>5V</v>
+        <v>3.9V</v>
       </c>
       <c r="G34" s="2" t="str">
         <f t="shared" si="1"/>

</xml_diff>